<commit_message>
first try for VA_senstivity plot
</commit_message>
<xml_diff>
--- a/CVX_Kenya/sens_Productivity increase due to 100% new machines (not spoiling the cerry)/case_0.005.xlsx
+++ b/CVX_Kenya/sens_Productivity increase due to 100% new machines (not spoiling the cerry)/case_0.005.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\payam\Documents\GitHub\CIVICS_Kenya\CVX_Kenya\sens_Productivity increase due to 100% new machines (not spoiling the cerry)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC259D51-036F-49E9-8416-7C71E245BC35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4424D37F-D7D6-4AD5-A8B6-C92BB2D240A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S" sheetId="1" r:id="rId1"/>

</xml_diff>